<commit_message>
cierre de cambios qmas 3 feb
</commit_message>
<xml_diff>
--- a/usuarios1.xlsx
+++ b/usuarios1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FLASH\flask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F7332F-BEF4-4F9F-8DC5-03F76BA85AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5135F78-A188-494F-AD5E-CB77BF6648CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2D155BBC-D73D-46F5-BE2C-B5665795BB38}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>numero_token</t>
   </si>
@@ -62,10 +62,7 @@
     <t>Claro TyT</t>
   </si>
   <si>
-    <t>Caren Lorena Gallego Peña</t>
-  </si>
-  <si>
-    <t>Michell Mesa</t>
+    <t>Stefany Jimenez</t>
   </si>
 </sst>
 </file>
@@ -101,9 +98,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -439,9 +435,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F80EB0-6B6A-4540-A740-E5FAA8D34F23}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -451,7 +449,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
@@ -475,7 +473,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1000983509</v>
+        <v>1000588257</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -487,37 +485,13 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1000983509</v>
-      </c>
-      <c r="F2" s="1" t="str">
+        <v>1000588257</v>
+      </c>
+      <c r="F2" t="str">
         <f>_xlfn.CONCAT(E2,"@qmas.com")</f>
-        <v>1000983509@qmas.com</v>
+        <v>1000588257@qmas.com</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1001315941</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>3114813698</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1001315941</v>
-      </c>
-      <c r="F3" s="1" t="str">
-        <f>_xlfn.CONCAT(E3,"@qmas.com")</f>
-        <v>1001315941@qmas.com</v>
-      </c>
-      <c r="G3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrega menu movil
</commit_message>
<xml_diff>
--- a/usuarios1.xlsx
+++ b/usuarios1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FLASH\flask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CF8BA0-8738-4AC8-B2C2-99718504A9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB854EEA-190F-42EF-B25D-8A4F1122BF26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2D155BBC-D73D-46F5-BE2C-B5665795BB38}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>numero_token</t>
   </si>
@@ -62,7 +62,58 @@
     <t>Claro TyT</t>
   </si>
   <si>
-    <t>Luisa Mozo</t>
+    <t>Laura Ximena Granados Ortiz</t>
+  </si>
+  <si>
+    <t>Cindy Natalia Gonzalez Gonzalez</t>
+  </si>
+  <si>
+    <t>Felipe Ipuz Toro</t>
+  </si>
+  <si>
+    <t>Sebastian Guzman Barbosa</t>
+  </si>
+  <si>
+    <t>Wilson Nicolas Fraile Briceño</t>
+  </si>
+  <si>
+    <t>Royer Santiago Soto</t>
+  </si>
+  <si>
+    <t>Esteven Eduardo Torres</t>
+  </si>
+  <si>
+    <t>Astrid Carolina Marin Otalora</t>
+  </si>
+  <si>
+    <t>Michael Steven Sutachan Paez</t>
+  </si>
+  <si>
+    <t>1070922246</t>
+  </si>
+  <si>
+    <t>1136882247</t>
+  </si>
+  <si>
+    <t>1053779508</t>
+  </si>
+  <si>
+    <t>1014285389</t>
+  </si>
+  <si>
+    <t>1020788095</t>
+  </si>
+  <si>
+    <t>1000733128</t>
+  </si>
+  <si>
+    <t>1021670403</t>
+  </si>
+  <si>
+    <t>1001068002</t>
+  </si>
+  <si>
+    <t>1000727443</t>
   </si>
 </sst>
 </file>
@@ -434,7 +485,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01F80EB0-6B6A-4540-A740-E5FAA8D34F23}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -469,26 +520,218 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1000132531</v>
+      <c r="A2" t="s">
+        <v>17</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
       <c r="C2">
-        <v>3114813698</v>
+        <v>3138311716</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>1000132531</v>
+      <c r="E2" t="s">
+        <v>17</v>
       </c>
       <c r="F2" t="str">
         <f>_xlfn.CONCAT(E2,"@qmas.com")</f>
-        <v>1000132531@qmas.com</v>
+        <v>1070922246@qmas.com</v>
       </c>
       <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>3138311716</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" ref="F3:F10" si="0">_xlfn.CONCAT(E3,"@qmas.com")</f>
+        <v>1136882247@qmas.com</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>3138311716</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>1053779508@qmas.com</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <v>3138311716</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>1014285389@qmas.com</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>3138311716</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>1020788095@qmas.com</v>
+      </c>
+      <c r="G6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>3138311716</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>1000733128@qmas.com</v>
+      </c>
+      <c r="G7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <v>3138311716</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>1021670403@qmas.com</v>
+      </c>
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>3138311716</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>1001068002@qmas.com</v>
+      </c>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>3138311716</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>1000727443@qmas.com</v>
+      </c>
+      <c r="G10" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>